<commit_message>
Add buttons and sections and very basic formatting
Added authentication buttons (like training)
Added hopes and dreams buttons
Updated plan
</commit_message>
<xml_diff>
--- a/wdi-proj2-plan.xlsx
+++ b/wdi-proj2-plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27260" windowHeight="13120" tabRatio="500"/>
+    <workbookView xWindow="1100" yWindow="1620" windowWidth="27260" windowHeight="16260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="task level" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="163">
   <si>
     <t>review controller files</t>
   </si>
@@ -451,12 +451,203 @@
   <si>
     <t>step</t>
   </si>
+  <si>
+    <t>After receiving the project prompt, decide what kind of app to make, and begin sketching some rough wireframes for how the front end will look and act.</t>
+  </si>
+  <si>
+    <t> Think about what kind of data your front-end will need from your back-end, and how that data will be used. Create an ERD.</t>
+  </si>
+  <si>
+    <t> Create two repos that your project will use, and add READMEs to both.</t>
+  </si>
+  <si>
+    <t> Create a simple front-end with HTML and CSS based (loosely) on your wireframes.</t>
+  </si>
+  <si>
+    <t> User our rails-api-template for your back-end. It already includes authentication.</t>
+  </si>
+  <si>
+    <r>
+      <t> After you have an ERD, check with a consultant to ensure your data model is appropriate for your goals. Then, build the models and migrations to represent this data. Test your models using the Rails console, and test your API endpoints using </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>curl</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>. You may also write automated tests in RSpec if you choose.</t>
+    </r>
+  </si>
+  <si>
+    <t> Before working on the front-end application, ensure all back-end endpoints work as expected. Knowing the back-end well will help you diagnose bugs on the front-end.</t>
+  </si>
+  <si>
+    <t> Write your front-end application using JavaScript, jQuery, and AJAX.</t>
+  </si>
+  <si>
+    <t> Test, commit, and deploy often! Test, commit, deploy! Test your deployments!</t>
+  </si>
+  <si>
+    <t> When main features are finished, begin working on stretch goals and icebox features.</t>
+  </si>
+  <si>
+    <t> Finish your documentation. Make it high-quality.</t>
+  </si>
+  <si>
+    <t>Tips</t>
+  </si>
+  <si>
+    <t>Begin with the end in mind. Know where you want to go by planning with wireframes and user stories, so you don't waste time designing and building things you don't need.</t>
+  </si>
+  <si>
+    <t>Remember that your backend environment is different from your browser environment – use tools to help you visualize it.</t>
+  </si>
+  <si>
+    <t>Don’t hesitate to write throwaway code to solve short term problems.</t>
+  </si>
+  <si>
+    <t>Read the docs for whatever technologies / frameworks / API’s that you use. Most of the time, there is a tutorial that you can follow, but not always, and learning to read documentation is crucial to your success as a developer.</t>
+  </si>
+  <si>
+    <r>
+      <t>Commit early, commit often.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t> As long as you do that, you don’t be afraid about breaking something, because you can always go back in time to a previous version. Always work on a branch!</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>User stories define what a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="16"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>user</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t> wants to accomplish with your application. It's tempting to just make them todo lists for what needs to get done, but if you keep them small and focused on the user's needs, it'll help you know what to build.</t>
+    </r>
+  </si>
+  <si>
+    <t>Write pseudocode before you write actual code. Thinking through the logic of something helps.</t>
+  </si>
+  <si>
+    <t>Finally, here are some resources that it might be good for you to look at/read about:</t>
+  </si>
+  <si>
+    <t>Heroku Documentation</t>
+  </si>
+  <si>
+    <t>Writing Good User Stories</t>
+  </si>
+  <si>
+    <t>Presenting Information Architecture</t>
+  </si>
+  <si>
+    <t>Good luck and happy hacking!</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>wednesday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>create section for authentication</t>
+  </si>
+  <si>
+    <t>add buttons for authentication</t>
+  </si>
+  <si>
+    <t>create section for hopes and dreams</t>
+  </si>
+  <si>
+    <t>add buttons for hopes and dreams</t>
+  </si>
+  <si>
+    <t>show all - default</t>
+  </si>
+  <si>
+    <t>show one</t>
+  </si>
+  <si>
+    <t>update one hope and dream</t>
+  </si>
+  <si>
+    <t>hide 1 hope and dream</t>
+  </si>
+  <si>
+    <t>remove 1 hope and dream completely</t>
+  </si>
+  <si>
+    <t>polish index.html</t>
+  </si>
+  <si>
+    <t>polish index.scss</t>
+  </si>
+  <si>
+    <t>polish handlebars</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>connect authent with back end</t>
+  </si>
+  <si>
+    <t>connect entries with back end</t>
+  </si>
+  <si>
+    <t>fix/continue with connection</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -481,6 +672,40 @@
       <color theme="1"/>
       <name val="Consolas"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF24292E"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF24292E"/>
+      <name val="Consolas"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF24292E"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF24292E"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="16"/>
+      <color rgb="FF24292E"/>
+      <name val="Helvetica"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -499,10 +724,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -515,8 +741,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -792,19 +1023,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A23" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A33" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="L48" sqref="L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.6640625" customWidth="1"/>
     <col min="3" max="3" width="41.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>114</v>
       </c>
@@ -812,162 +1044,204 @@
         <v>29</v>
       </c>
       <c r="D1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="5">
         <v>42850</v>
       </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="5">
         <v>42850</v>
       </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4" s="5">
         <v>42850</v>
       </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E5" s="5">
         <v>42851</v>
       </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
       <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="5">
         <v>42851</v>
       </c>
-      <c r="E6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E7" s="5">
         <v>42851</v>
       </c>
-      <c r="E7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E8" s="5">
         <v>42852</v>
       </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>1</v>
       </c>
       <c r="D10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E10" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D11" t="s">
+        <v>142</v>
+      </c>
+      <c r="E11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
+        <v>142</v>
+      </c>
+      <c r="E12" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D13" t="s">
+        <v>142</v>
+      </c>
+      <c r="E13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D14" t="s">
+        <v>142</v>
+      </c>
+      <c r="E14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>7</v>
       </c>
@@ -977,143 +1251,191 @@
       <c r="C15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" t="s">
+        <v>142</v>
+      </c>
+      <c r="E15" s="5">
         <v>42852</v>
       </c>
-      <c r="E15" t="s">
-        <v>28</v>
-      </c>
       <c r="F15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>8</v>
       </c>
       <c r="B16" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C17" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" t="s">
+        <v>142</v>
+      </c>
+      <c r="E17" s="5">
         <v>42852</v>
       </c>
-      <c r="E17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C18" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" t="s">
+        <v>142</v>
+      </c>
+      <c r="E18" s="5">
         <v>42852</v>
       </c>
-      <c r="E18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C19" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E19" s="5">
         <v>42852</v>
       </c>
-      <c r="E19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C20" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" t="s">
+        <v>142</v>
+      </c>
+      <c r="E20" s="5">
         <v>42852</v>
       </c>
-      <c r="E20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C21" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" t="s">
+        <v>142</v>
+      </c>
+      <c r="E21" s="5">
         <v>42852</v>
       </c>
-      <c r="E21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C22" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" t="s">
+        <v>142</v>
+      </c>
+      <c r="E22" s="5">
         <v>42852</v>
       </c>
-      <c r="E22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C23" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E23" s="5">
         <v>42852</v>
       </c>
-      <c r="E23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C24" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D24" s="5">
-        <v>42852</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>142</v>
+      </c>
+      <c r="E24" s="5">
+        <v>42853</v>
+      </c>
+      <c r="F24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C25" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" t="s">
+        <v>142</v>
+      </c>
+      <c r="E25" s="5">
         <v>42852</v>
       </c>
-      <c r="E25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>9</v>
       </c>
       <c r="B26" t="s">
         <v>95</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" t="s">
+        <v>142</v>
+      </c>
+      <c r="E26" s="5">
         <v>42852</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>113</v>
       </c>
       <c r="B27" t="s">
         <v>101</v>
       </c>
-      <c r="D27" s="5">
-        <v>42852</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>141</v>
+      </c>
+      <c r="E27" s="5">
+        <v>42853</v>
+      </c>
+      <c r="F27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>15</v>
       </c>
@@ -1121,84 +1443,276 @@
         <v>23</v>
       </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="5">
-        <v>42852</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="D28" t="s">
+        <v>141</v>
+      </c>
+      <c r="E28" s="5">
+        <v>42853</v>
+      </c>
+      <c r="F28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E29" s="5">
+        <v>42853</v>
+      </c>
+      <c r="F29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E30" s="5">
+        <v>42853</v>
+      </c>
+      <c r="F30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>149</v>
+      </c>
+      <c r="E33" s="5">
+        <v>42853</v>
+      </c>
+      <c r="F33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>150</v>
+      </c>
+      <c r="E34" s="5">
+        <v>42853</v>
+      </c>
+      <c r="F34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41">
         <v>16</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B41" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="5">
-        <v>42852</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="C41" s="1"/>
+      <c r="D41" t="s">
+        <v>141</v>
+      </c>
+      <c r="E41" s="5">
+        <v>42853</v>
+      </c>
+      <c r="F41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42">
         <v>17</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B42" t="s">
         <v>96</v>
       </c>
-      <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="C42" s="1"/>
+      <c r="D42" t="s">
+        <v>141</v>
+      </c>
+      <c r="E42" s="5">
+        <v>42853</v>
+      </c>
+      <c r="F42" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43">
         <v>18</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B43" t="s">
+        <v>160</v>
+      </c>
+      <c r="D43" t="s">
+        <v>141</v>
+      </c>
+      <c r="E43" s="5">
+        <v>42853</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>19</v>
+      </c>
+      <c r="B44" t="s">
+        <v>161</v>
+      </c>
+      <c r="D44" t="s">
+        <v>141</v>
+      </c>
+      <c r="E44" s="5">
+        <v>42853</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>20</v>
+      </c>
+      <c r="B46" t="s">
+        <v>162</v>
+      </c>
+      <c r="D46" t="s">
+        <v>159</v>
+      </c>
+      <c r="E46" s="5">
+        <v>42854</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>21</v>
+      </c>
+      <c r="B47" t="s">
+        <v>156</v>
+      </c>
+      <c r="E47" s="5">
+        <v>42854</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>22</v>
+      </c>
+      <c r="B48" t="s">
+        <v>157</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" t="s">
+        <v>141</v>
+      </c>
+      <c r="E48" s="5">
+        <v>42854</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>23</v>
+      </c>
+      <c r="B49" t="s">
+        <v>158</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" t="s">
+        <v>141</v>
+      </c>
+      <c r="E49" s="5">
+        <v>42854</v>
+      </c>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>24</v>
+      </c>
+      <c r="B50" t="s">
         <v>111</v>
       </c>
-      <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>19</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="C50" s="1"/>
+      <c r="D50" t="s">
+        <v>146</v>
+      </c>
+      <c r="E50" s="5">
+        <v>42854</v>
+      </c>
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>25</v>
+      </c>
+      <c r="B51" t="s">
         <v>112</v>
       </c>
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>20</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="C51" s="1"/>
+      <c r="D51" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" s="5">
+        <v>42854</v>
+      </c>
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D53" s="1"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>26</v>
+      </c>
+      <c r="B58" t="s">
         <v>97</v>
       </c>
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>21</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="C58" s="1"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>27</v>
+      </c>
+      <c r="B59" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>22</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="C59" s="1"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>28</v>
+      </c>
+      <c r="B60" t="s">
         <v>99</v>
       </c>
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>23</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="C60" s="1"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>29</v>
+      </c>
+      <c r="B61" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1327,120 +1841,210 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:A27"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="J2" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="J3" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="J4" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="J5" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="J6" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="J7" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="J8" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="J9" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="J10" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="J11" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="J12" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="23" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="J15" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="J16" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="J17" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="J18" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="J19" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="J20" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="J21" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="J22" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="J23" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="J24" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="J25" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="J26" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="J27" s="11" t="s">
+        <v>138</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J6" r:id="rId1"/>
+    <hyperlink ref="J24" r:id="rId2"/>
+    <hyperlink ref="J25" r:id="rId3"/>
+    <hyperlink ref="J26" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add files for authent n edit some existing w cmmnts
</commit_message>
<xml_diff>
--- a/wdi-proj2-plan.xlsx
+++ b/wdi-proj2-plan.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="165">
   <si>
     <t>review controller files</t>
   </si>
@@ -641,6 +641,12 @@
   </si>
   <si>
     <t>fix/continue with connection</t>
+  </si>
+  <si>
+    <t>add functionality for authentication</t>
+  </si>
+  <si>
+    <t>add functionality for hopes and dreams</t>
   </si>
 </sst>
 </file>
@@ -1025,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A33" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="L48" sqref="L48"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A20" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1475,6 +1481,11 @@
         <v>28</v>
       </c>
     </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>163</v>
+      </c>
+    </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
         <v>149</v>
@@ -1520,6 +1531,11 @@
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
         <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Move img folder and add img to html
</commit_message>
<xml_diff>
--- a/wdi-proj2-plan.xlsx
+++ b/wdi-proj2-plan.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="170">
   <si>
     <t>review controller files</t>
   </si>
@@ -647,6 +647,21 @@
   </si>
   <si>
     <t>add functionality for hopes and dreams</t>
+  </si>
+  <si>
+    <t>sign up functionality</t>
+  </si>
+  <si>
+    <t>sign in functionality</t>
+  </si>
+  <si>
+    <t>sign out functionality</t>
+  </si>
+  <si>
+    <t>change password functionality</t>
+  </si>
+  <si>
+    <t>Friday/Saturday</t>
   </si>
 </sst>
 </file>
@@ -713,12 +728,18 @@
       <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA6FF8E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -734,7 +755,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -751,6 +772,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -758,6 +784,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFA6FF8E"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1029,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A20" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A37" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1425,19 +1456,20 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="A27" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="D27" t="s">
+      <c r="C27" s="12"/>
+      <c r="D27" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="13">
         <v>42853</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="12" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1463,6 +1495,9 @@
       <c r="C29" t="s">
         <v>147</v>
       </c>
+      <c r="D29" t="s">
+        <v>141</v>
+      </c>
       <c r="E29" s="5">
         <v>42853</v>
       </c>
@@ -1474,6 +1509,9 @@
       <c r="C30" t="s">
         <v>148</v>
       </c>
+      <c r="D30" t="s">
+        <v>141</v>
+      </c>
       <c r="E30" s="5">
         <v>42853</v>
       </c>
@@ -1482,255 +1520,447 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>16</v>
+      </c>
       <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" t="s">
+        <v>141</v>
+      </c>
+      <c r="E31" s="5">
+        <v>42853</v>
+      </c>
+      <c r="F31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="12">
+        <v>17</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="E32" s="13">
+        <v>42853</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="12">
+        <v>18</v>
+      </c>
+      <c r="B33" s="12" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C33" t="s">
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="E34" s="13">
+        <v>42853</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="E35" s="13">
+        <v>42853</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="E36" s="13">
+        <v>42853</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="E37" s="13">
+        <v>42853</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="12">
+        <v>19</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="E38" s="13">
+        <v>42853</v>
+      </c>
+      <c r="F38" s="12"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="E33" s="5">
+      <c r="D39" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="E39" s="13">
+        <v>42854</v>
+      </c>
+      <c r="F39" s="12"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="E40" s="13">
+        <v>42854</v>
+      </c>
+      <c r="F40" s="12"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="E41" s="13">
+        <v>42854</v>
+      </c>
+      <c r="F41" s="12"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="E42" s="13">
+        <v>42854</v>
+      </c>
+      <c r="F42" s="12"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="E43" s="13">
+        <v>42854</v>
+      </c>
+      <c r="F43" s="12"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="E44" s="13">
+        <v>42854</v>
+      </c>
+      <c r="F44" s="12"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="E45" s="13">
+        <v>42854</v>
+      </c>
+      <c r="F45" s="12"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="12">
+        <v>20</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="E52" s="13">
         <v>42853</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F52" s="12"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="12">
+        <v>21</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="E53" s="13">
+        <v>42853</v>
+      </c>
+      <c r="F53" s="12"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="12"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="12">
+        <v>22</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E55" s="13">
+        <v>42854</v>
+      </c>
+      <c r="F55" s="12"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="12">
+        <v>23</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="13">
+        <v>42854</v>
+      </c>
+      <c r="F56" s="12"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="12">
+        <v>24</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C57" s="14"/>
+      <c r="D57" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="E57" s="13">
+        <v>42854</v>
+      </c>
+      <c r="F57" s="12"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="12">
+        <v>25</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="C58" s="14"/>
+      <c r="D58" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="E58" s="13">
+        <v>42854</v>
+      </c>
+      <c r="F58" s="13"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="12">
+        <v>26</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C59" s="14"/>
+      <c r="D59" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E59" s="13">
+        <v>42854</v>
+      </c>
+      <c r="F59" s="13"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="12">
+        <v>27</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C60" s="14"/>
+      <c r="D60" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E60" s="13">
+        <v>42854</v>
+      </c>
+      <c r="F60" s="13"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="12"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="12">
         <v>28</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C34" t="s">
-        <v>150</v>
-      </c>
-      <c r="E34" s="5">
-        <v>42853</v>
-      </c>
-      <c r="F34" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C35" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C36" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C37" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C38" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C39" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>16</v>
-      </c>
-      <c r="B41" t="s">
-        <v>24</v>
-      </c>
-      <c r="C41" s="1"/>
-      <c r="D41" t="s">
-        <v>141</v>
-      </c>
-      <c r="E41" s="5">
-        <v>42853</v>
-      </c>
-      <c r="F41" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>17</v>
-      </c>
-      <c r="B42" t="s">
-        <v>96</v>
-      </c>
-      <c r="C42" s="1"/>
-      <c r="D42" t="s">
-        <v>141</v>
-      </c>
-      <c r="E42" s="5">
-        <v>42853</v>
-      </c>
-      <c r="F42" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>18</v>
-      </c>
-      <c r="B43" t="s">
-        <v>160</v>
-      </c>
-      <c r="D43" t="s">
-        <v>141</v>
-      </c>
-      <c r="E43" s="5">
-        <v>42853</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>19</v>
-      </c>
-      <c r="B44" t="s">
-        <v>161</v>
-      </c>
-      <c r="D44" t="s">
-        <v>141</v>
-      </c>
-      <c r="E44" s="5">
-        <v>42853</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>20</v>
-      </c>
-      <c r="B46" t="s">
-        <v>162</v>
-      </c>
-      <c r="D46" t="s">
-        <v>159</v>
-      </c>
-      <c r="E46" s="5">
-        <v>42854</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>21</v>
-      </c>
-      <c r="B47" t="s">
-        <v>156</v>
-      </c>
-      <c r="E47" s="5">
-        <v>42854</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>22</v>
-      </c>
-      <c r="B48" t="s">
-        <v>157</v>
-      </c>
-      <c r="C48" s="1"/>
-      <c r="D48" t="s">
-        <v>141</v>
-      </c>
-      <c r="E48" s="5">
-        <v>42854</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>23</v>
-      </c>
-      <c r="B49" t="s">
-        <v>158</v>
-      </c>
-      <c r="C49" s="1"/>
-      <c r="D49" t="s">
-        <v>141</v>
-      </c>
-      <c r="E49" s="5">
-        <v>42854</v>
-      </c>
-      <c r="F49" s="5"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>24</v>
-      </c>
-      <c r="B50" t="s">
-        <v>111</v>
-      </c>
-      <c r="C50" s="1"/>
-      <c r="D50" t="s">
-        <v>146</v>
-      </c>
-      <c r="E50" s="5">
-        <v>42854</v>
-      </c>
-      <c r="F50" s="5"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>25</v>
-      </c>
-      <c r="B51" t="s">
-        <v>112</v>
-      </c>
-      <c r="C51" s="1"/>
-      <c r="D51" t="s">
-        <v>146</v>
-      </c>
-      <c r="E51" s="5">
-        <v>42854</v>
-      </c>
-      <c r="F51" s="5"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D53" s="1"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>26</v>
-      </c>
-      <c r="B58" t="s">
+      <c r="B62" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C58" s="1"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>27</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="C62" s="12"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="12">
+        <v>29</v>
+      </c>
+      <c r="B63" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="C59" s="1"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>28</v>
-      </c>
-      <c r="B60" t="s">
+      <c r="C63" s="12"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="12">
+        <v>30</v>
+      </c>
+      <c r="B64" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="C60" s="1"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>29</v>
-      </c>
-      <c r="B61" t="s">
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="12">
+        <v>31</v>
+      </c>
+      <c r="B65" s="12" t="s">
         <v>100</v>
       </c>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="12"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="12"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="12"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C69" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update plan with status
</commit_message>
<xml_diff>
--- a/wdi-proj2-plan.xlsx
+++ b/wdi-proj2-plan.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="170">
   <si>
     <t>review controller files</t>
   </si>
@@ -755,7 +755,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -777,6 +777,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1062,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A37" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A28" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1648,32 +1650,36 @@
       <c r="F38" s="12"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12" t="s">
+      <c r="A39" s="15"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="D39" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="E39" s="13">
+      <c r="E39" s="16">
         <v>42854</v>
       </c>
-      <c r="F39" s="12"/>
+      <c r="F39" s="15" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12" t="s">
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="D40" s="12" t="s">
+      <c r="D40" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="E40" s="13">
+      <c r="E40" s="16">
         <v>42854</v>
       </c>
-      <c r="F40" s="12"/>
+      <c r="F40" s="15" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="12"/>
@@ -1687,7 +1693,9 @@
       <c r="E41" s="13">
         <v>42854</v>
       </c>
-      <c r="F41" s="12"/>
+      <c r="F41" s="12" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="12"/>
@@ -1701,7 +1709,9 @@
       <c r="E42" s="13">
         <v>42854</v>
       </c>
-      <c r="F42" s="12"/>
+      <c r="F42" s="12" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="12"/>
@@ -1715,7 +1725,9 @@
       <c r="E43" s="13">
         <v>42854</v>
       </c>
-      <c r="F43" s="12"/>
+      <c r="F43" s="12" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="12"/>
@@ -1729,7 +1741,9 @@
       <c r="E44" s="13">
         <v>42854</v>
       </c>
-      <c r="F44" s="12"/>
+      <c r="F44" s="12" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="12"/>
@@ -1743,7 +1757,9 @@
       <c r="E45" s="13">
         <v>42854</v>
       </c>
-      <c r="F45" s="12"/>
+      <c r="F45" s="12" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="12">

</xml_diff>

<commit_message>
Add code for get entry
still working on creating to test
</commit_message>
<xml_diff>
--- a/wdi-proj2-plan.xlsx
+++ b/wdi-proj2-plan.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="171">
   <si>
     <t>review controller files</t>
   </si>
@@ -663,12 +663,15 @@
   <si>
     <t>Friday/Saturday</t>
   </si>
+  <si>
+    <t>this is working with curl req in prod but not displaying my console.logs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -727,6 +730,14 @@
       <color rgb="FF24292E"/>
       <name val="Helvetica"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -755,7 +766,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -779,6 +790,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1062,10 +1074,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A28" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:F40"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A21" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1076,22 +1088,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="17" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1557,7 +1570,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="12">
         <v>18</v>
       </c>
@@ -1569,7 +1582,7 @@
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="12"/>
       <c r="B34" s="12"/>
       <c r="C34" s="12" t="s">
@@ -1584,8 +1597,16 @@
       <c r="F34" s="12" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="12"/>
       <c r="B35" s="12"/>
       <c r="C35" s="12" t="s">
@@ -1600,8 +1621,16 @@
       <c r="F35" s="12" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="12"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
@@ -1616,8 +1645,16 @@
       <c r="F36" s="12" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="12"/>
       <c r="B37" s="12"/>
       <c r="C37" s="12" t="s">
@@ -1632,8 +1669,16 @@
       <c r="F37" s="12" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="12">
         <v>19</v>
       </c>
@@ -1649,7 +1694,7 @@
       </c>
       <c r="F38" s="12"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="15"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15" t="s">
@@ -1665,7 +1710,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="15"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15" t="s">
@@ -1681,7 +1726,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="12"/>
       <c r="B41" s="12"/>
       <c r="C41" s="12" t="s">
@@ -1697,7 +1742,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="12"/>
       <c r="B42" s="12"/>
       <c r="C42" s="12" t="s">
@@ -1713,7 +1758,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
       <c r="C43" s="12" t="s">
@@ -1729,7 +1774,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="12"/>
       <c r="B44" s="12"/>
       <c r="C44" s="12" t="s">
@@ -1745,7 +1790,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="12"/>
       <c r="B45" s="12"/>
       <c r="C45" s="12" t="s">

</xml_diff>

<commit_message>
Update authentication functionality - working
Updated click handling
Updated appear/disappear
Updated so that token is displayed
</commit_message>
<xml_diff>
--- a/wdi-proj2-plan.xlsx
+++ b/wdi-proj2-plan.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="170">
   <si>
     <t>review controller files</t>
   </si>
@@ -662,9 +662,6 @@
   </si>
   <si>
     <t>Friday/Saturday</t>
-  </si>
-  <si>
-    <t>this is working with curl req in prod but not displaying my console.logs</t>
   </si>
 </sst>
 </file>
@@ -1076,8 +1073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A21" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1571,35 +1568,33 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="12">
+      <c r="A33" s="15">
         <v>18</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12" t="s">
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="E34" s="13">
-        <v>42853</v>
-      </c>
-      <c r="F34" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="G34" s="15" t="s">
-        <v>170</v>
-      </c>
+      <c r="E34" s="16">
+        <v>42855</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G34" s="15"/>
       <c r="H34" s="15"/>
       <c r="I34" s="15"/>
       <c r="J34" s="15"/>
@@ -1607,23 +1602,21 @@
       <c r="L34" s="15"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12" t="s">
+      <c r="A35" s="15"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="E35" s="13">
-        <v>42853</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="G35" s="15" t="s">
-        <v>170</v>
-      </c>
+      <c r="E35" s="16">
+        <v>42855</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G35" s="15"/>
       <c r="H35" s="15"/>
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
@@ -1631,23 +1624,21 @@
       <c r="L35" s="15"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12" t="s">
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="E36" s="13">
-        <v>42853</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="G36" s="15" t="s">
-        <v>170</v>
-      </c>
+      <c r="E36" s="16">
+        <v>42855</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" s="15"/>
       <c r="H36" s="15"/>
       <c r="I36" s="15"/>
       <c r="J36" s="15"/>
@@ -1655,23 +1646,21 @@
       <c r="L36" s="15"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12" t="s">
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="E37" s="13">
-        <v>42853</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="G37" s="15" t="s">
-        <v>170</v>
-      </c>
+      <c r="E37" s="16">
+        <v>42855</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G37" s="15"/>
       <c r="H37" s="15"/>
       <c r="I37" s="15"/>
       <c r="J37" s="15"/>

</xml_diff>

<commit_message>
Add updates to plan, show One
</commit_message>
<xml_diff>
--- a/wdi-proj2-plan.xlsx
+++ b/wdi-proj2-plan.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="195">
   <si>
     <t>review controller files</t>
   </si>
@@ -398,9 +398,6 @@
     <t>create js files/handlebars</t>
   </si>
   <si>
-    <t>test authentication</t>
-  </si>
-  <si>
     <t>test entrie CRUD from UI</t>
   </si>
   <si>
@@ -664,7 +661,82 @@
     <t>Friday/Saturday</t>
   </si>
   <si>
-    <t>ISSUE</t>
+    <t>create new</t>
+  </si>
+  <si>
+    <t>test authentication from UI</t>
+  </si>
+  <si>
+    <t>Deliverables</t>
+  </si>
+  <si>
+    <t>A working full-stack application, built by you, hosted somewhere on the internet.</t>
+  </si>
+  <si>
+    <t>Two Github repos (one for your front-end and one for your back-end), with frequent commits dating back to the very beginning of the project. Each repo will need a README.md file with a link to the other repo. Your front-end repo's README should also have</t>
+  </si>
+  <si>
+    <t>An explanation of the what the app does and how it works, the approach taken in building it, and any unsolved problems that you hit.</t>
+  </si>
+  <si>
+    <t>User stories written for your app.</t>
+  </si>
+  <si>
+    <t>At least one wireframe (or a link to one) that you've created to plan out your app.</t>
+  </si>
+  <si>
+    <t>A link to the live application.</t>
+  </si>
+  <si>
+    <t>Your app must</t>
+  </si>
+  <si>
+    <t>Your app must not</t>
+  </si>
+  <si>
+    <t>Have any obvious user-facing errors</t>
+  </si>
+  <si>
+    <t>Rely on refreshing the page for any functionality.</t>
+  </si>
+  <si>
+    <t>Bonus</t>
+  </si>
+  <si>
+    <t>Once (and only once) you've satisfied the core requirements, here are some additional goals that you can shoot for:</t>
+  </si>
+  <si>
+    <t>Incorporate Bootstrap, Handlebars, or some other front-end tool.</t>
+  </si>
+  <si>
+    <t>Interact with third-party APIs and integrate them into your app.</t>
+  </si>
+  <si>
+    <t>Put some extra thought and effort into visual and UI design.</t>
+  </si>
+  <si>
+    <t>Have an API that is securely accessible by your browser app, built using frameworks covered in class.</t>
+  </si>
+  <si>
+    <t>Create at least 4 RESTful routes for handling GET, POST, PUT/PATCH, and DELETE requests. Any actions which change data must be authenticated, and the data must be "owned" by the user performing the change.</t>
+  </si>
+  <si>
+    <t>Utilize an ORM to create a database table structure and interact with data</t>
+  </si>
+  <si>
+    <t>Use a front-end Javascript app to communicate with your API (both read and write) and render data that it receives in the browser.</t>
+  </si>
+  <si>
+    <t>Have semantically clean HTML and CSS</t>
+  </si>
+  <si>
+    <t>Be deployed online, so that it is accessible to the public</t>
+  </si>
+  <si>
+    <t>Be linked in your pinned repositories on your GitHub profile page</t>
+  </si>
+  <si>
+    <t>make legends, links.  When click on links, forms display</t>
   </si>
 </sst>
 </file>
@@ -766,7 +838,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -791,6 +863,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1074,10 +1150,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L69"/>
+  <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A27" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A33" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1089,14 +1165,14 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>29</v>
       </c>
       <c r="C1" s="17"/>
       <c r="D1" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>30</v>
@@ -1116,7 +1192,7 @@
         <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E2" s="5">
         <v>42850</v>
@@ -1133,7 +1209,7 @@
         <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E3" s="5">
         <v>42850</v>
@@ -1150,7 +1226,7 @@
         <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E4" s="5">
         <v>42850</v>
@@ -1167,7 +1243,7 @@
         <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E5" s="5">
         <v>42851</v>
@@ -1187,7 +1263,7 @@
         <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E6" s="5">
         <v>42851</v>
@@ -1204,7 +1280,7 @@
         <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E7" s="5">
         <v>42851</v>
@@ -1221,7 +1297,7 @@
         <v>85</v>
       </c>
       <c r="D8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E8" s="5">
         <v>42852</v>
@@ -1235,7 +1311,7 @@
         <v>86</v>
       </c>
       <c r="D9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1243,7 +1319,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E10" t="s">
         <v>87</v>
@@ -1254,7 +1330,7 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E11" t="s">
         <v>88</v>
@@ -1265,7 +1341,7 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E12" t="s">
         <v>89</v>
@@ -1276,7 +1352,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E13" t="s">
         <v>90</v>
@@ -1287,7 +1363,7 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E14" t="s">
         <v>91</v>
@@ -1304,7 +1380,7 @@
         <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E15" s="5">
         <v>42852</v>
@@ -1324,15 +1400,15 @@
         <v>94</v>
       </c>
       <c r="D16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C17" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E17" s="5">
         <v>42852</v>
@@ -1343,10 +1419,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C18" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E18" s="5">
         <v>42852</v>
@@ -1357,10 +1433,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C19" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E19" s="5">
         <v>42852</v>
@@ -1371,10 +1447,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C20" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E20" s="5">
         <v>42852</v>
@@ -1385,10 +1461,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C21" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E21" s="5">
         <v>42852</v>
@@ -1399,10 +1475,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C22" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E22" s="5">
         <v>42852</v>
@@ -1413,10 +1489,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C23" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E23" s="5">
         <v>42852</v>
@@ -1427,10 +1503,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C24" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E24" s="5">
         <v>42853</v>
@@ -1441,10 +1517,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C25" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E25" s="5">
         <v>42852</v>
@@ -1461,7 +1537,7 @@
         <v>95</v>
       </c>
       <c r="D26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E26" s="5">
         <v>42852</v>
@@ -1472,20 +1548,20 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E27" s="13">
         <v>42853</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1497,7 +1573,7 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E28" s="5">
         <v>42853</v>
@@ -1508,10 +1584,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E29" s="5">
         <v>42853</v>
@@ -1522,10 +1598,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E30" s="5">
         <v>42853</v>
@@ -1543,7 +1619,7 @@
       </c>
       <c r="C31" s="1"/>
       <c r="D31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E31" s="5">
         <v>42853</v>
@@ -1561,13 +1637,13 @@
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E32" s="13">
         <v>42853</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -1575,7 +1651,7 @@
         <v>18</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="15"/>
@@ -1590,10 +1666,10 @@
       <c r="A34" s="15"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E34" s="16">
         <v>42856</v>
@@ -1606,18 +1682,16 @@
       <c r="I34" s="15"/>
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
-      <c r="L34" s="15" t="s">
-        <v>170</v>
-      </c>
+      <c r="L34" s="15"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="15"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E35" s="16">
         <v>42856</v>
@@ -1630,18 +1704,16 @@
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
-      <c r="L35" s="15" t="s">
-        <v>170</v>
-      </c>
+      <c r="L35" s="15"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="15"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E36" s="16">
         <v>42856</v>
@@ -1654,18 +1726,16 @@
       <c r="I36" s="15"/>
       <c r="J36" s="15"/>
       <c r="K36" s="15"/>
-      <c r="L36" s="15" t="s">
-        <v>170</v>
-      </c>
+      <c r="L36" s="15"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="15"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E37" s="16">
         <v>42856</v>
@@ -1678,20 +1748,18 @@
       <c r="I37" s="15"/>
       <c r="J37" s="15"/>
       <c r="K37" s="15"/>
-      <c r="L37" s="15" t="s">
-        <v>170</v>
-      </c>
+      <c r="L37" s="15"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="12">
         <v>19</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C38" s="12"/>
       <c r="D38" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E38" s="13">
         <v>42853</v>
@@ -1702,10 +1770,10 @@
       <c r="A39" s="15"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E39" s="16">
         <v>42854</v>
@@ -1718,10 +1786,10 @@
       <c r="A40" s="15"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E40" s="16">
         <v>42854</v>
@@ -1731,147 +1799,167 @@
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="E41" s="13">
-        <v>42854</v>
-      </c>
-      <c r="F41" s="12" t="s">
-        <v>139</v>
+      <c r="A41" s="15"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="E41" s="16">
+        <v>42856</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="12"/>
       <c r="B42" s="12"/>
       <c r="C42" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E42" s="13">
         <v>42854</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="D43" s="12" t="s">
+      <c r="A43" s="15"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="E43" s="13">
-        <v>42854</v>
-      </c>
-      <c r="F43" s="12" t="s">
-        <v>139</v>
+      <c r="D43" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="E43" s="16">
+        <v>42856</v>
+      </c>
+      <c r="F43" s="15" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="12"/>
       <c r="B44" s="12"/>
       <c r="C44" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E44" s="13">
         <v>42854</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="12"/>
       <c r="B45" s="12"/>
       <c r="C45" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E45" s="13">
         <v>42854</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="12">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="E46" s="13">
+        <v>42854</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="15">
         <v>20</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B52" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="E52" s="16">
+        <v>42856</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="15">
+        <v>21</v>
+      </c>
+      <c r="B53" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="E52" s="13">
-        <v>42853</v>
-      </c>
-      <c r="F52" s="12"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="12">
-        <v>21</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="E53" s="13">
-        <v>42853</v>
-      </c>
-      <c r="F53" s="12"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="12"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C53" s="15"/>
+      <c r="D53" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="E53" s="16">
+        <v>42856</v>
+      </c>
+      <c r="F53" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="15"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="12">
         <v>22</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C55" s="12"/>
       <c r="D55" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E55" s="13">
         <v>42854</v>
       </c>
       <c r="F55" s="12"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="12">
         <v>23</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C56" s="12"/>
       <c r="D56" s="12"/>
@@ -1880,71 +1968,74 @@
       </c>
       <c r="F56" s="12"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="12">
         <v>24</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C57" s="14"/>
       <c r="D57" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E57" s="13">
         <v>42854</v>
       </c>
       <c r="F57" s="12"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G57" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="12">
         <v>25</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C58" s="14"/>
       <c r="D58" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E58" s="13">
         <v>42854</v>
       </c>
       <c r="F58" s="13"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="12">
         <v>26</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C59" s="14"/>
       <c r="D59" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E59" s="13">
         <v>42854</v>
       </c>
       <c r="F59" s="13"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="12">
         <v>27</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C60" s="14"/>
       <c r="D60" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E60" s="13">
         <v>42854</v>
       </c>
       <c r="F60" s="13"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="12"/>
       <c r="B61" s="12"/>
       <c r="C61" s="14"/>
@@ -1952,55 +2043,60 @@
       <c r="E61" s="12"/>
       <c r="F61" s="12"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="12">
-        <v>28</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C62" s="12"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" s="15">
+        <v>28</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C62" s="15"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="16">
+        <v>42856</v>
+      </c>
+      <c r="F62" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G62" s="15"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="12">
         <v>29</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C63" s="12"/>
       <c r="D63" s="12"/>
       <c r="E63" s="12"/>
       <c r="F63" s="12"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="12">
         <v>30</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C64" s="12"/>
       <c r="D64" s="12"/>
       <c r="E64" s="12"/>
       <c r="F64" s="12"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="12">
         <v>31</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C65" s="12"/>
       <c r="D65" s="12"/>
       <c r="E65" s="12"/>
       <c r="F65" s="12"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="12"/>
       <c r="B66" s="12"/>
       <c r="C66" s="12"/>
@@ -2008,7 +2104,7 @@
       <c r="E66" s="12"/>
       <c r="F66" s="12"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="12"/>
       <c r="B67" s="12"/>
       <c r="C67" s="14"/>
@@ -2016,16 +2112,348 @@
       <c r="E67" s="12"/>
       <c r="F67" s="12"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="12"/>
-      <c r="B68" s="12"/>
-      <c r="C68" s="14"/>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" s="12">
+        <v>31</v>
+      </c>
+      <c r="B68" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C68" s="12"/>
       <c r="D68" s="12"/>
       <c r="E68" s="12"/>
       <c r="F68" s="12"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C69" s="1"/>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" s="12"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" s="12"/>
+      <c r="B70" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="C70" s="12"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" s="12"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" s="12"/>
+      <c r="B72" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C72" s="12"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" s="12"/>
+      <c r="B73" s="12"/>
+      <c r="C73" s="12"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="12"/>
+      <c r="G73" s="12"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" s="12"/>
+      <c r="B74" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="12"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" s="12"/>
+      <c r="B75" s="12"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="12"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" s="12"/>
+      <c r="B76" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" s="12"/>
+      <c r="B77" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="C77" s="12"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
+      <c r="G77" s="12"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" s="12"/>
+      <c r="B78" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+      <c r="G78" s="12"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" s="12"/>
+      <c r="B79" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" s="12"/>
+      <c r="B80" s="12"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+      <c r="G80" s="12"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" s="12"/>
+      <c r="B81" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="C81" s="12"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="12"/>
+      <c r="G81" s="12"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" s="12"/>
+      <c r="B82" s="12"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="12"/>
+      <c r="F82" s="12"/>
+      <c r="G82" s="12"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83" s="12"/>
+      <c r="B83" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="C83" s="12"/>
+      <c r="D83" s="12"/>
+      <c r="E83" s="12"/>
+      <c r="F83" s="12"/>
+      <c r="G83" s="12"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" s="12"/>
+      <c r="B84" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="C84" s="12"/>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+      <c r="G84" s="12"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" s="12"/>
+      <c r="B85" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="12"/>
+      <c r="F85" s="12"/>
+      <c r="G85" s="12"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86" s="12"/>
+      <c r="B86" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C86" s="12"/>
+      <c r="D86" s="12"/>
+      <c r="E86" s="12"/>
+      <c r="F86" s="12"/>
+      <c r="G86" s="12"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" s="12"/>
+      <c r="B87" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="C87" s="12"/>
+      <c r="D87" s="12"/>
+      <c r="E87" s="12"/>
+      <c r="F87" s="12"/>
+      <c r="G87" s="12"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88" s="12"/>
+      <c r="B88" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="C88" s="12"/>
+      <c r="D88" s="12"/>
+      <c r="E88" s="12"/>
+      <c r="F88" s="12"/>
+      <c r="G88" s="12"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89" s="12"/>
+      <c r="B89" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="C89" s="12"/>
+      <c r="D89" s="12"/>
+      <c r="E89" s="12"/>
+      <c r="F89" s="12"/>
+      <c r="G89" s="12"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90" s="12"/>
+      <c r="B90" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C90" s="12"/>
+      <c r="D90" s="12"/>
+      <c r="E90" s="12"/>
+      <c r="F90" s="12"/>
+      <c r="G90" s="12"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91" s="12"/>
+      <c r="B91" s="12"/>
+      <c r="C91" s="12"/>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="12"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92" s="12"/>
+      <c r="B92" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="C92" s="12"/>
+      <c r="D92" s="12"/>
+      <c r="E92" s="12"/>
+      <c r="F92" s="12"/>
+      <c r="G92" s="12"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A93" s="12"/>
+      <c r="B93" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="C93" s="12"/>
+      <c r="D93" s="12"/>
+      <c r="E93" s="12"/>
+      <c r="F93" s="12"/>
+      <c r="G93" s="12"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A94" s="12"/>
+      <c r="B94" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="C94" s="12"/>
+      <c r="D94" s="12"/>
+      <c r="E94" s="12"/>
+      <c r="F94" s="12"/>
+      <c r="G94" s="12"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A95" s="12"/>
+      <c r="B95" s="12"/>
+      <c r="C95" s="12"/>
+      <c r="D95" s="12"/>
+      <c r="E95" s="12"/>
+      <c r="F95" s="12"/>
+      <c r="G95" s="12"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A96" s="12"/>
+      <c r="B96" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="C96" s="12"/>
+      <c r="D96" s="12"/>
+      <c r="E96" s="12"/>
+      <c r="F96" s="12"/>
+      <c r="G96" s="12"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A97" s="12"/>
+      <c r="B97" s="12"/>
+      <c r="C97" s="12"/>
+      <c r="D97" s="12"/>
+      <c r="E97" s="12"/>
+      <c r="F97" s="12"/>
+      <c r="G97" s="12"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A98" s="12"/>
+      <c r="B98" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="C98" s="12"/>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="12"/>
+      <c r="G98" s="12"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A99" s="12"/>
+      <c r="B99" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="C99" s="12"/>
+      <c r="D99" s="12"/>
+      <c r="E99" s="12"/>
+      <c r="F99" s="12"/>
+      <c r="G99" s="12"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A100" s="12"/>
+      <c r="B100" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="C100" s="12"/>
+      <c r="D100" s="12"/>
+      <c r="E100" s="12"/>
+      <c r="F100" s="12"/>
+      <c r="G100" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2167,7 +2595,7 @@
     </row>
     <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="J2" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.25">
@@ -2175,12 +2603,12 @@
         <v>37</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="J4" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="21" x14ac:dyDescent="0.25">
@@ -2188,7 +2616,7 @@
         <v>40</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -2196,7 +2624,7 @@
         <v>41</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="21" x14ac:dyDescent="0.25">
@@ -2204,7 +2632,7 @@
         <v>42</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="21" x14ac:dyDescent="0.25">
@@ -2212,7 +2640,7 @@
         <v>43</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="21" x14ac:dyDescent="0.25">
@@ -2220,17 +2648,17 @@
         <v>44</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="J10" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="J11" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="21" x14ac:dyDescent="0.25">
@@ -2238,7 +2666,7 @@
         <v>80</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="19" x14ac:dyDescent="0.25">
@@ -2256,7 +2684,7 @@
         <v>83</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="21" x14ac:dyDescent="0.25">
@@ -2264,17 +2692,17 @@
         <v>84</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="J17" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="J18" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="21" x14ac:dyDescent="0.25">
@@ -2282,7 +2710,7 @@
         <v>18</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="21" x14ac:dyDescent="0.25">
@@ -2290,7 +2718,7 @@
         <v>5</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="21" x14ac:dyDescent="0.25">
@@ -2298,7 +2726,7 @@
         <v>6</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="21" x14ac:dyDescent="0.25">
@@ -2306,7 +2734,7 @@
         <v>7</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="21" x14ac:dyDescent="0.25">
@@ -2314,7 +2742,7 @@
         <v>19</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -2322,7 +2750,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -2330,7 +2758,7 @@
         <v>21</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -2338,7 +2766,7 @@
         <v>5</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="21" x14ac:dyDescent="0.25">
@@ -2346,7 +2774,7 @@
         <v>22</v>
       </c>
       <c r="J27" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add project documentation - README, plan, screenshot
</commit_message>
<xml_diff>
--- a/wdi-proj2-plan.xlsx
+++ b/wdi-proj2-plan.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="173">
   <si>
     <t>review controller files</t>
   </si>
@@ -659,6 +659,18 @@
   </si>
   <si>
     <t>create new hope or dream</t>
+  </si>
+  <si>
+    <t>not started</t>
+  </si>
+  <si>
+    <t>optional</t>
+  </si>
+  <si>
+    <t>somewhat</t>
+  </si>
+  <si>
+    <t>subtask</t>
   </si>
 </sst>
 </file>
@@ -760,7 +772,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -770,7 +782,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -778,15 +789,31 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1071,105 +1098,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L69"/>
+  <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A30" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A41" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52:F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
     <col min="3" max="3" width="41.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="17" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17" t="s">
+      <c r="C1" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="17">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="20">
         <v>42850</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="17" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="17">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>33</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="20">
         <v>42850</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="17" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="17">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>35</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="20">
         <v>42850</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="17" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="17">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>38</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="20">
         <v>42851</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="17" t="s">
         <v>28</v>
       </c>
       <c r="G5" t="s">
@@ -1177,53 +1208,53 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="17">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="20">
         <v>42851</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="17" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="17">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>45</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="20">
         <v>42851</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="17" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="17">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>85</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="20">
         <v>42852</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="17" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1231,7 +1262,7 @@
       <c r="C9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="17" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1239,10 +1270,10 @@
       <c r="C10" t="s">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="17" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1250,10 +1281,10 @@
       <c r="C11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="17" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1261,10 +1292,10 @@
       <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="17" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1272,10 +1303,10 @@
       <c r="C13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="17" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1283,15 +1314,15 @@
       <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="17" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="17">
         <v>7</v>
       </c>
       <c r="B15" t="s">
@@ -1300,13 +1331,13 @@
       <c r="C15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="20">
         <v>42852</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="17" t="s">
         <v>28</v>
       </c>
       <c r="G15" t="s">
@@ -1314,13 +1345,13 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="A16" s="17">
         <v>8</v>
       </c>
       <c r="B16" t="s">
         <v>94</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="17" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1328,13 +1359,13 @@
       <c r="C17" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="20">
         <v>42852</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="17" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1342,13 +1373,13 @@
       <c r="C18" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="20">
         <v>42852</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="17" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1356,13 +1387,13 @@
       <c r="C19" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="20">
         <v>42852</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="17" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1370,13 +1401,13 @@
       <c r="C20" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="20">
         <v>42852</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="17" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1384,13 +1415,13 @@
       <c r="C21" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="20">
         <v>42852</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="17" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1398,13 +1429,13 @@
       <c r="C22" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="20">
         <v>42852</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="17" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1412,13 +1443,13 @@
       <c r="C23" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="20">
         <v>42852</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="17" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1426,13 +1457,13 @@
       <c r="C24" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="20">
         <v>42853</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="17" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1440,66 +1471,66 @@
       <c r="C25" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="20">
         <v>42852</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="17" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="A26" s="17">
         <v>9</v>
       </c>
       <c r="B26" t="s">
         <v>95</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="20">
         <v>42852</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="17" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="E27" s="13">
+      <c r="C27" s="13"/>
+      <c r="D27" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="E27" s="21">
         <v>42853</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="19" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="A28" s="17">
         <v>15</v>
       </c>
       <c r="B28" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="1"/>
-      <c r="D28" t="s">
+      <c r="D28" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="20">
         <v>42853</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="17" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1507,13 +1538,13 @@
       <c r="C29" t="s">
         <v>147</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="20">
         <v>42853</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="17" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1521,490 +1552,517 @@
       <c r="C30" t="s">
         <v>148</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="20">
         <v>42853</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="17" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="A31" s="17">
         <v>16</v>
       </c>
       <c r="B31" t="s">
         <v>24</v>
       </c>
       <c r="C31" s="1"/>
-      <c r="D31" t="s">
+      <c r="D31" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31" s="20">
         <v>42853</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="17" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="12">
+      <c r="A32" s="19">
         <v>17</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="12" t="s">
+      <c r="C32" s="15"/>
+      <c r="D32" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="E32" s="13">
-        <v>42853</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>139</v>
+      <c r="E32" s="21">
+        <v>42855</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="15">
+      <c r="A33" s="19">
         <v>18</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15" t="s">
+      <c r="A34" s="19"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="E34" s="16">
+      <c r="E34" s="21">
         <v>42855</v>
       </c>
-      <c r="F34" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
+      <c r="F34" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="15"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15" t="s">
+      <c r="A35" s="19"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="E35" s="16">
+      <c r="E35" s="21">
         <v>42855</v>
       </c>
-      <c r="F35" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
+      <c r="F35" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15" t="s">
+      <c r="A36" s="19"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="E36" s="16">
+      <c r="E36" s="21">
         <v>42855</v>
       </c>
-      <c r="F36" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
+      <c r="F36" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="15"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15" t="s">
+      <c r="A37" s="19"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="E37" s="16">
+      <c r="E37" s="21">
         <v>42855</v>
       </c>
-      <c r="F37" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
+      <c r="F37" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="12">
+      <c r="A38" s="19">
         <v>19</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12" t="s">
+      <c r="C38" s="13"/>
+      <c r="D38" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="E38" s="13">
-        <v>42853</v>
-      </c>
-      <c r="F38" s="12"/>
+      <c r="E38" s="21">
+        <v>42857</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="15"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15" t="s">
+      <c r="A39" s="19"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="D39" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="E39" s="16">
+      <c r="E39" s="21">
         <v>42854</v>
       </c>
-      <c r="F39" s="15" t="s">
+      <c r="F39" s="19" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15" t="s">
+      <c r="A40" s="19"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="E40" s="16">
+      <c r="E40" s="21">
         <v>42854</v>
       </c>
-      <c r="F40" s="15" t="s">
+      <c r="F40" s="19" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="15"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15" t="s">
+      <c r="A41" s="19"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="E41" s="16">
+      <c r="E41" s="21">
         <v>42856</v>
       </c>
-      <c r="F41" s="15" t="s">
+      <c r="F41" s="19" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="15"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15" t="s">
+      <c r="A42" s="19"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D42" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="E42" s="16">
+      <c r="E42" s="21">
         <v>42856</v>
       </c>
-      <c r="F42" s="15" t="s">
+      <c r="F42" s="19" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12" t="s">
+      <c r="A43" s="19"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="D43" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="E43" s="13">
-        <v>42854</v>
-      </c>
-      <c r="F43" s="12" t="s">
-        <v>139</v>
+      <c r="E43" s="21">
+        <v>42857</v>
+      </c>
+      <c r="F43" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12" t="s">
+      <c r="A44" s="19"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="D44" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="E44" s="13">
-        <v>42854</v>
-      </c>
-      <c r="F44" s="12" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="15">
+      <c r="E44" s="21">
+        <v>42857</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" s="19">
         <v>20</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B45" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15" t="s">
+      <c r="C45" s="13"/>
+      <c r="D45" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="E52" s="16">
+      <c r="E45" s="21">
         <v>42856</v>
       </c>
-      <c r="F52" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="15">
+      <c r="F45" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" s="19">
         <v>21</v>
       </c>
-      <c r="B53" s="15" t="s">
+      <c r="B46" s="13" t="s">
         <v>159</v>
       </c>
+      <c r="C46" s="13"/>
+      <c r="D46" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="E46" s="21">
+        <v>42856</v>
+      </c>
+      <c r="F46" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" s="19"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48" s="19">
+        <v>22</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C48" s="13"/>
+      <c r="D48" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="E48" s="21">
+        <v>42856</v>
+      </c>
+      <c r="F48" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="19">
+        <v>23</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C49" s="13"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="21">
+        <v>42857</v>
+      </c>
+      <c r="F49" s="19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="19">
+        <v>24</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="C50" s="15"/>
+      <c r="D50" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="E50" s="21">
+        <v>42857</v>
+      </c>
+      <c r="F50" s="19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="19">
+        <v>25</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C51" s="15"/>
+      <c r="D51" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="E51" s="21">
+        <v>42857</v>
+      </c>
+      <c r="F51" s="19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="18">
+        <v>26</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C52" s="12"/>
+      <c r="D52" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="E52" s="21">
+        <v>42857</v>
+      </c>
+      <c r="F52" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="19">
+        <v>27</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>112</v>
+      </c>
       <c r="C53" s="15"/>
-      <c r="D53" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="E53" s="16">
+      <c r="D53" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="E53" s="21">
+        <v>42857</v>
+      </c>
+      <c r="F53" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G53" s="13"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="19"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="19">
+        <v>28</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" s="13"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="21">
         <v>42856</v>
       </c>
-      <c r="F53" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="15"/>
-      <c r="B54" s="15"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="15"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="15">
-        <v>22</v>
-      </c>
-      <c r="B55" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="E55" s="16">
+      <c r="F55" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="19">
+        <v>29</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C56" s="13"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="21">
+        <v>42857</v>
+      </c>
+      <c r="F56" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="18">
+        <v>30</v>
+      </c>
+      <c r="B57" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" s="11"/>
+      <c r="D57" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="19">
+        <v>31</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C58" s="13"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="21">
         <v>42856</v>
       </c>
-      <c r="F55" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="12">
-        <v>23</v>
-      </c>
-      <c r="B56" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="13">
-        <v>42854</v>
-      </c>
-      <c r="F56" s="12"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="12">
-        <v>24</v>
-      </c>
-      <c r="B57" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="C57" s="14"/>
-      <c r="D57" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="E57" s="13">
-        <v>42854</v>
-      </c>
-      <c r="F57" s="12"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="12">
-        <v>25</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="C58" s="14"/>
-      <c r="D58" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="E58" s="13">
-        <v>42854</v>
-      </c>
-      <c r="F58" s="13"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="12">
-        <v>26</v>
-      </c>
-      <c r="B59" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C59" s="14"/>
-      <c r="D59" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="E59" s="13">
-        <v>42854</v>
-      </c>
-      <c r="F59" s="13"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="12">
-        <v>27</v>
-      </c>
-      <c r="B60" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="C60" s="14"/>
-      <c r="D60" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="E60" s="13">
-        <v>42854</v>
-      </c>
-      <c r="F60" s="13"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="12"/>
-      <c r="B61" s="12"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="15">
-        <v>28</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C62" s="15"/>
-      <c r="D62" s="18"/>
-      <c r="E62" s="16">
-        <v>42856</v>
-      </c>
-      <c r="F62" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="12">
-        <v>29</v>
-      </c>
-      <c r="B63" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="12">
-        <v>30</v>
-      </c>
-      <c r="B64" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="C64" s="12"/>
-      <c r="D64" s="12"/>
-      <c r="E64" s="12"/>
-      <c r="F64" s="12"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="12">
-        <v>31</v>
-      </c>
-      <c r="B65" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C65" s="12"/>
-      <c r="D65" s="12"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="12"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="12"/>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
-      <c r="E66" s="12"/>
-      <c r="F66" s="12"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="12"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="14"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="12"/>
-      <c r="F67" s="12"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="12"/>
-      <c r="B68" s="12"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="12"/>
-      <c r="E68" s="12"/>
-      <c r="F68" s="12"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C69" s="1"/>
+      <c r="F58" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="19"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="19"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="19"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="19"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" s="19"/>
+      <c r="B61" s="13"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="19"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C62" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2134,7 +2192,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2145,7 +2203,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2153,12 +2211,12 @@
       <c r="A3" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="7" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="7" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2166,7 +2224,7 @@
       <c r="A5" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="7" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2174,7 +2232,7 @@
       <c r="B6" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="8" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2182,7 +2240,7 @@
       <c r="B7" t="s">
         <v>42</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="7" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2190,7 +2248,7 @@
       <c r="B8" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="7" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2198,61 +2256,61 @@
       <c r="B9" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="7" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="7" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="J11" s="8" t="s">
+      <c r="J11" s="7" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" s="7" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="23" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="J15" s="10" t="s">
+      <c r="J15" s="9" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J16" s="7" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="J17" s="8" t="s">
+      <c r="J17" s="7" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="J18" s="8" t="s">
+      <c r="J18" s="7" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2260,7 +2318,7 @@
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="J19" s="7" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2268,7 +2326,7 @@
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J20" s="11" t="s">
+      <c r="J20" s="10" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2276,7 +2334,7 @@
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J21" s="8" t="s">
+      <c r="J21" s="7" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2284,7 +2342,7 @@
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J22" s="8" t="s">
+      <c r="J22" s="7" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2292,7 +2350,7 @@
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J23" s="8" t="s">
+      <c r="J23" s="7" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2300,7 +2358,7 @@
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="9" t="s">
+      <c r="J24" s="8" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2308,7 +2366,7 @@
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J25" s="9" t="s">
+      <c r="J25" s="8" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2316,7 +2374,7 @@
       <c r="A26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J26" s="9" t="s">
+      <c r="J26" s="8" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2324,7 +2382,7 @@
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J27" s="11" t="s">
+      <c r="J27" s="10" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2373,7 +2431,7 @@
       <c r="F2" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>